<commit_message>
WADNR-1939 Add Report Center functionality from Project Firma - Updated documentation, removing unavailable fields - Removed unused model classes
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C619BF68-8429-4371-AC1F-5349D8788985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244CD9C8-3EED-41D4-8350-91A52B9FF258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17985" yWindow="3690" windowWidth="38370" windowHeight="23370" activeTab="7" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="12324" yWindow="1044" windowWidth="37860" windowHeight="18744" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,8 @@
     <sheet name="ProjectContact" sheetId="4" r:id="rId4"/>
     <sheet name="Person" sheetId="2" r:id="rId5"/>
     <sheet name="Organization" sheetId="3" r:id="rId6"/>
-    <sheet name="ProjectStatus" sheetId="7" r:id="rId7"/>
-    <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId8"/>
-    <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId9"/>
-    <sheet name="TechnicalAssistanceRequest" sheetId="10" r:id="rId10"/>
+    <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId7"/>
+    <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="233">
   <si>
     <t>Description of Field</t>
   </si>
@@ -134,24 +132,12 @@
     <t>Estimated Total Cost</t>
   </si>
   <si>
-    <t>Secured Funding</t>
-  </si>
-  <si>
-    <t>Targeted Funding</t>
-  </si>
-  <si>
-    <t>No Funding Source Identified</t>
-  </si>
-  <si>
     <t>Project ID</t>
   </si>
   <si>
     <t>Project Last Updated</t>
   </si>
   <si>
-    <t>Final Status Update Status</t>
-  </si>
-  <si>
     <t>&lt;%= project.ImplementationStartYear %&gt;</t>
   </si>
   <si>
@@ -173,19 +159,7 @@
     <t>&lt;%= project.FundingType %&gt;</t>
   </si>
   <si>
-    <t>&lt;%= project.SecuredFunding %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= project.TargetedFunding %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= project.NoFundingSourceIdentified %&gt;</t>
-  </si>
-  <si>
     <t>&lt;%= project.ProjectID %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= project.FinalStatusUpdateStatus %&gt;</t>
   </si>
   <si>
     <t>End Foreach</t>
@@ -559,18 +533,6 @@
     <t>&lt;%= Model.ReportTitle %&gt;</t>
   </si>
   <si>
-    <t>Current Project Status</t>
-  </si>
-  <si>
-    <t>Current Project Status Color</t>
-  </si>
-  <si>
-    <t>&lt;%= project.CurrentProjectStatus %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= project.CurrentProjectStatusColor %&gt;</t>
-  </si>
-  <si>
     <t>ProjectImage</t>
   </si>
   <si>
@@ -797,159 +759,6 @@
   </si>
   <si>
     <t>ProjectContact</t>
-  </si>
-  <si>
-    <t>ProjectStatus(es)</t>
-  </si>
-  <si>
-    <t>Get All Project Statuses From the Last Week</t>
-  </si>
-  <si>
-    <t>&lt;% var projectStatuses = project.GetAllProjectStatusesFromTheLastWeek(); %&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Returns a list of ProjectStatus models from the previous week starting on Monday up to the current day. (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ProjectStatus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tab) </t>
-    </r>
-  </si>
-  <si>
-    <t>Get Project Statuses from the Last Week</t>
-  </si>
-  <si>
-    <t>Returns a list of ProjectStatus models from the previous week starting on Monday up to the current day.</t>
-  </si>
-  <si>
-    <t>&lt;% if(projectStatuses.Any()) { ?&gt;</t>
-  </si>
-  <si>
-    <t>If there are project statuses</t>
-  </si>
-  <si>
-    <t>ProjectStatus in Project Statuses</t>
-  </si>
-  <si>
-    <t>&lt;% foreach(var projectStatus in projectStatuses) { %&gt;</t>
-  </si>
-  <si>
-    <t>End the Project Statuses loop</t>
-  </si>
-  <si>
-    <t>ProjectStatus</t>
-  </si>
-  <si>
-    <t>Returns the Date of the Status Update</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.UpdateStatus %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.CreatePersonName %&gt;</t>
-  </si>
-  <si>
-    <t>Create Person Name</t>
-  </si>
-  <si>
-    <t>Update Date</t>
-  </si>
-  <si>
-    <t>Create Date</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.CreateDate %&gt;</t>
-  </si>
-  <si>
-    <t>Returns the full name (First then Last) of the user that created the status</t>
-  </si>
-  <si>
-    <t>Returns the date the Status was created</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.LastEditedPersonName %&gt;</t>
-  </si>
-  <si>
-    <t>Returns the full name (First then Last) of the last user to edit the status. If no edits, it will return the CreatePersonName.</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.LastEditedDate %&gt;</t>
-  </si>
-  <si>
-    <t>Last Edited Person Name</t>
-  </si>
-  <si>
-    <t>Last Edited Date</t>
-  </si>
-  <si>
-    <t>Project Status Comment</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusComment %&gt;</t>
-  </si>
-  <si>
-    <t>Project Status Display Name</t>
-  </si>
-  <si>
-    <t>Project Status Color</t>
-  </si>
-  <si>
-    <t>Project Status Description</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusDisplayName %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusColor %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusDescription %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusRecentActivities %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusUpcomingActivities %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= projectStatus.ProjectStatusRisksOrIssues %&gt;</t>
-  </si>
-  <si>
-    <t>Field is only accessible in the Reclamation client branch</t>
-  </si>
-  <si>
-    <t>Returns the selected status</t>
-  </si>
-  <si>
-    <t>Returns the color value of the selected status</t>
-  </si>
-  <si>
-    <t>Returns the description of the selected status</t>
-  </si>
-  <si>
-    <t>*Project Status Recent Activities</t>
-  </si>
-  <si>
-    <t>*Project Status Upcoming Activities</t>
-  </si>
-  <si>
-    <t>*Project Status Risks Or Issues</t>
   </si>
   <si>
     <t>Get All Project Reported Performance Measure Values</t>
@@ -1121,9 +930,6 @@
     <t>ProjectExpectedPerformanceMeasure(s)</t>
   </si>
   <si>
-    <t>Get all Project Technical Assistance Requests</t>
-  </si>
-  <si>
     <t>Get All Project Expected Performance Measure values</t>
   </si>
   <si>
@@ -1131,147 +937,6 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>&lt;%= var technicalAssistanceRequests = project.GetProjectTechnicalAssistanceRequests(); %&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Returns a list of ProjectTechnicalAssistanceRequest models (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>TechnicalAssistanceRequest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tab)</t>
-    </r>
-  </si>
-  <si>
-    <t>ProjectTechnicalAssistanceRequest(s)</t>
-  </si>
-  <si>
-    <t>ProjectTechnicalAssistanceRequest</t>
-  </si>
-  <si>
-    <t>If there are Project Technical Assistance Requests</t>
-  </si>
-  <si>
-    <t>Start Project Technical Assistance Requests loop</t>
-  </si>
-  <si>
-    <t>Assigned Person</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Hours Requested</t>
-  </si>
-  <si>
-    <t>Hours Allocated</t>
-  </si>
-  <si>
-    <t>Hours Provided</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Dollar Value Decimal Value</t>
-  </si>
-  <si>
-    <t>Dollar Value String (text) Value</t>
-  </si>
-  <si>
-    <t>Returns a list of ProjectTechnicalAssistanceRequest models</t>
-  </si>
-  <si>
-    <t>&lt;% if(technicalAssistanceRequests.Any()) { ?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;% foreach(var technicalAssistanceRequest in technicalAssistanceRequests) { %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.FiscalYear %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.Notes %&gt;</t>
-  </si>
-  <si>
-    <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.Type %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursRequested %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursAllocated %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.HoursPrivded %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.DollarValueDecimal %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= technicalAssistanceRequest.DollarValueString %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;% var assignedPerson =  technicalAssistanceRequest.AssignedPerson; %&gt;</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Returns a single Person model (see </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Person</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tab)</t>
-    </r>
-  </si>
-  <si>
-    <t>Returns the raw decimal value (e.g. 10.05) useful for adding/calculations</t>
-  </si>
-  <si>
-    <t>Returns a dollar formatted text value (e.g. $10.05) useful for simply displaying dollar value</t>
-  </si>
-  <si>
-    <t>End the Project Technical Assistance Requests loop</t>
-  </si>
-  <si>
-    <t>Idaho Soil &amp; Water Conservation Commission Only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTE: This model is only applicable to Idaho Soil &amp; Water Conservation Commission's ProjectFirma Instance. </t>
   </si>
   <si>
     <t>Entering subcategory information is optional for Expected Performance Measures, so this may return an empty string</t>
@@ -1284,7 +949,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,13 +1042,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1391,16 +1049,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1497,11 +1147,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1512,82 +1157,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FB0E11C-9AD4-467E-ABE3-B008EF9DCF04}"/>
   </cellStyles>
@@ -1901,23 +1538,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="100.5703125" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" customWidth="1"/>
+    <col min="5" max="5" width="100.5546875" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1932,829 +1569,440 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="47"/>
-    </row>
-    <row r="4" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47" t="s">
+      <c r="E3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="46"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-    </row>
-    <row r="5" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52" t="s">
+      <c r="E5" s="51"/>
+      <c r="F5" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52" t="s">
+      <c r="D6" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52" t="s">
+      <c r="E7" s="51"/>
+      <c r="F7" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52" t="s">
+      <c r="E8" s="51"/>
+      <c r="F8" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52" t="s">
+      <c r="E9" s="51"/>
+      <c r="F9" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="52" t="s">
+      <c r="E12" s="51"/>
+      <c r="F12" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="51" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="47"/>
+      <c r="B28" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="52" t="s">
+      <c r="C28" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="52" t="s">
+      <c r="D28" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
-        <v>282</v>
-      </c>
-      <c r="B27" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>261</v>
-      </c>
-      <c r="E27" s="52" t="s">
-        <v>263</v>
-      </c>
-      <c r="F27" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>283</v>
-      </c>
-      <c r="B28" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>285</v>
-      </c>
-      <c r="D28" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="E28" s="52" t="s">
-        <v>264</v>
-      </c>
-      <c r="F28" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="56" t="s">
-        <v>128</v>
-      </c>
-      <c r="F30" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="D32" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="B33" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="56" t="s">
-        <v>200</v>
-      </c>
-      <c r="D33" s="53" t="s">
-        <v>201</v>
-      </c>
-      <c r="E33" s="56" t="s">
-        <v>202</v>
-      </c>
-      <c r="F33" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="D34" s="53" t="s">
-        <v>147</v>
-      </c>
-      <c r="E34" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="F34" s="52" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
-        <v>290</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="56" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" s="52" t="s">
-        <v>288</v>
-      </c>
-      <c r="E35" s="56" t="s">
-        <v>289</v>
-      </c>
-      <c r="F35" s="60" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD1C35-1AF3-403F-B823-0BA284571615}">
-  <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="72" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>320</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-    </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="42"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24" t="s">
-        <v>301</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>313</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="44"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2766,16 +2014,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2790,7 +2038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2053,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2818,406 +2066,406 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E34" s="44"/>
     </row>
@@ -3234,16 +2482,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3258,7 +2506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -3271,11 +2519,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3288,172 +2536,172 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E16" s="44"/>
     </row>
@@ -3470,16 +2718,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3494,8 +2742,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="43" t="s">
@@ -3509,8 +2757,8 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
       </c>
@@ -3520,170 +2768,170 @@
       <c r="D3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
       <c r="B16" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="51"/>
+        <v>42</v>
+      </c>
+      <c r="E16" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3699,16 +2947,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3723,7 +2971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3738,7 +2986,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3751,172 +2999,172 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>114</v>
-      </c>
       <c r="E13" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E16" s="44"/>
     </row>
@@ -3933,16 +3181,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3957,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3972,7 +3220,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3985,174 +3233,174 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E16" s="44"/>
     </row>
@@ -4162,23 +3410,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9A00D5-E39F-4947-BF8A-C9BC6B110727}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="97" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4193,307 +3441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="43"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="58"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="58"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="E15" s="58" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="E17" s="58" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="59"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="59"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="51"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4506,11 +3454,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4523,153 +3471,153 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>282</v>
+        <v>226</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>245</v>
+        <v>189</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>266</v>
+        <v>210</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>265</v>
+        <v>209</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>255</v>
+        <v>199</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>256</v>
+        <v>200</v>
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>257</v>
+        <v>201</v>
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>259</v>
+        <v>203</v>
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>253</v>
+        <v>197</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="44"/>
     </row>
@@ -4678,7 +3626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -4686,16 +3634,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4710,7 +3658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4723,11 +3671,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4740,146 +3688,146 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>283</v>
+        <v>227</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>267</v>
+        <v>211</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>262</v>
+        <v>206</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>275</v>
+        <v>219</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>270</v>
+        <v>214</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>276</v>
+        <v>220</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>271</v>
+        <v>215</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>277</v>
+        <v>221</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>278</v>
+        <v>222</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>279</v>
+        <v>223</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>280</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>281</v>
+        <v>225</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>274</v>
+        <v>218</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E14" s="44"/>
     </row>

</xml_diff>

<commit_message>
WADNR-1939 Add Report Center functionality from Project Firma - Fixed ? found in documentation which were causing errors for report templates
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244CD9C8-3EED-41D4-8350-91A52B9FF258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A754BBDD-BDA7-4099-A25A-427D17E143AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12324" yWindow="1044" windowWidth="37860" windowHeight="18744" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="7800" yWindow="1344" windowWidth="37860" windowHeight="18744" activeTab="1" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -617,9 +617,6 @@
     <t>Get All Project Images</t>
   </si>
   <si>
-    <t>&lt;% if(projectImages.Any()) { ?&gt;</t>
-  </si>
-  <si>
     <t>If there are Project Images</t>
   </si>
   <si>
@@ -671,9 +668,6 @@
     <t>If there are Project Images with the "Before" timing</t>
   </si>
   <si>
-    <t>&lt;% if(beforeImages.Any()) { ?&gt;</t>
-  </si>
-  <si>
     <t>&lt;% foreach(var beforeImage in beforeImages) { %&gt;</t>
   </si>
   <si>
@@ -696,9 +690,6 @@
   </si>
   <si>
     <t>Returns a single ProjectImage model. Returns null if none are set for the project</t>
-  </si>
-  <si>
-    <t>&lt;% if(projectKeyPhoto != null) { ?&gt;</t>
   </si>
   <si>
     <t>If a Project Key Photo was retrieved</t>
@@ -943,6 +934,15 @@
   </si>
   <si>
     <t>Entering values is optional for Expected Performance Measures, so this may return an empty string</t>
+  </si>
+  <si>
+    <t>&lt;% if(projectImages.Any()) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% if(beforeImages.Any()) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% if(projectKeyPhoto != null) { %&gt;</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1569,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1827,7 +1827,7 @@
         <v>92</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1843,47 +1843,47 @@
         <v>95</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="51" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B21" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E21" s="51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="51" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B22" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
         <v>119</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1923,7 +1923,7 @@
         <v>120</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1937,18 +1937,18 @@
         <v>130</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E25" s="55" t="s">
         <v>133</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="55" t="s">
         <v>5</v>
@@ -1963,18 +1963,18 @@
         <v>134</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D27" s="52" t="s">
         <v>135</v>
@@ -1983,7 +1983,7 @@
         <v>136</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B737C5F2-D331-4EC0-AE50-ADE7E7050ACA}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
@@ -2089,10 +2089,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -2102,10 +2102,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="E6" s="15"/>
     </row>
@@ -2115,10 +2115,10 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -2126,10 +2126,10 @@
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -2137,10 +2137,10 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="25"/>
     </row>
@@ -2148,39 +2148,39 @@
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>172</v>
-      </c>
       <c r="E11" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>151</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2189,7 +2189,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>42</v>
@@ -2202,7 +2202,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>42</v>
@@ -2211,19 +2211,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>135</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2232,10 +2232,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>157</v>
+        <v>231</v>
       </c>
       <c r="E16" s="38"/>
     </row>
@@ -2245,10 +2245,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E17" s="38"/>
     </row>
@@ -2258,10 +2258,10 @@
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E18" s="25"/>
     </row>
@@ -2269,10 +2269,10 @@
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E19" s="25"/>
     </row>
@@ -2280,10 +2280,10 @@
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E20" s="25"/>
     </row>
@@ -2291,39 +2291,39 @@
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2332,7 +2332,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>42</v>
@@ -2345,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>42</v>
@@ -2363,10 +2363,10 @@
         <v>130</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2375,10 +2375,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>166</v>
+        <v>232</v>
       </c>
       <c r="E27" s="15"/>
     </row>
@@ -2388,10 +2388,10 @@
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E28" s="25"/>
     </row>
@@ -2399,10 +2399,10 @@
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E29" s="25"/>
     </row>
@@ -2410,10 +2410,10 @@
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E30" s="25"/>
     </row>
@@ -2421,26 +2421,26 @@
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2449,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>42</v>
@@ -2471,6 +2471,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2815,7 +2816,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24" t="s">
@@ -3473,19 +3474,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3494,10 +3495,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -3507,23 +3508,23 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -3531,10 +3532,10 @@
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -3542,10 +3543,10 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E9" s="28"/>
     </row>
@@ -3553,10 +3554,10 @@
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E10" s="29"/>
     </row>
@@ -3564,10 +3565,10 @@
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -3575,10 +3576,10 @@
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E12" s="25"/>
     </row>
@@ -3588,7 +3589,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>42</v>
@@ -3690,19 +3691,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3711,10 +3712,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -3724,23 +3725,23 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -3748,10 +3749,10 @@
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -3759,36 +3760,36 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E11" s="25"/>
     </row>
@@ -3798,7 +3799,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
WADNR-1989 Add IPR and Invoice fields to report generator updating excel doc adding Get functions to get child elements
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\wadnrforesthealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A754BBDD-BDA7-4099-A25A-427D17E143AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74906FC8-FC48-404A-9898-712FAA7B14A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="1344" windowWidth="37860" windowHeight="18744" activeTab="1" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="642" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Organization" sheetId="3" r:id="rId6"/>
     <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId7"/>
     <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId8"/>
+    <sheet name="InvoicePaymentRequest" sheetId="10" r:id="rId9"/>
+    <sheet name="Invoice" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="307">
   <si>
     <t>Description of Field</t>
   </si>
@@ -943,6 +945,228 @@
   </si>
   <si>
     <t>&lt;% if(projectKeyPhoto != null) { %&gt;</t>
+  </si>
+  <si>
+    <t>InvoicePaymentRequest(s)</t>
+  </si>
+  <si>
+    <t>Returns a list of InvoicePaymentRequest models (see InvoicePaymentRequest tab)</t>
+  </si>
+  <si>
+    <t>WADNR</t>
+  </si>
+  <si>
+    <t>InvoicePaymentRequests</t>
+  </si>
+  <si>
+    <t>Get all Invoice Payment Requests</t>
+  </si>
+  <si>
+    <t>&lt;% var invoicePaymentRequests = project.GetInvoicePaymentRequests(); %&gt;</t>
+  </si>
+  <si>
+    <t>Get All Invoice Payment Requests</t>
+  </si>
+  <si>
+    <t>Returns a list of InvoicePaymentRequest models</t>
+  </si>
+  <si>
+    <t>If there are Invoice Payment Requests</t>
+  </si>
+  <si>
+    <t>Invoice Payment Request in Invoice Payment Requests</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var invoicePaymentRequest in invoicePaymentRequests) { %&gt;</t>
+  </si>
+  <si>
+    <t>InvoicePaymentRequest</t>
+  </si>
+  <si>
+    <t>VendorName</t>
+  </si>
+  <si>
+    <t>VendorNumber</t>
+  </si>
+  <si>
+    <t>VendorAddressLine1</t>
+  </si>
+  <si>
+    <t>VendorAddressLine2</t>
+  </si>
+  <si>
+    <t>VendorAddressLine3</t>
+  </si>
+  <si>
+    <t>VendorCity</t>
+  </si>
+  <si>
+    <t>VendorState</t>
+  </si>
+  <si>
+    <t>VendorZip</t>
+  </si>
+  <si>
+    <t>PreparedByPerson</t>
+  </si>
+  <si>
+    <t>PurchaseAuthority</t>
+  </si>
+  <si>
+    <t>DUNS</t>
+  </si>
+  <si>
+    <t>InvoicePaymentRequestDate</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>&lt;% if(invoicePaymentRequests.Any()) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorNumber %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorAddressLine1 %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorAddressLine2 %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorAddressLine3 %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorCity %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorState %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorZip %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.PreparedByPerson %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.PurchaseAuthority %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.DUNS %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.InvoicePaymentRequestDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.Notes %&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of Invoice models (see invoice tab)</t>
+  </si>
+  <si>
+    <t>&lt;% var invoices = invoicePaymentRequest.GetInvoices(); %&gt;</t>
+  </si>
+  <si>
+    <t>End the Invoice Payment Requests loop</t>
+  </si>
+  <si>
+    <t>If there are Invoices</t>
+  </si>
+  <si>
+    <t>&lt;% if(invoices.Any()) { %&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of Invoice models</t>
+  </si>
+  <si>
+    <t>Invoice in Invoices</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var invoice in invoices) { %&gt;</t>
+  </si>
+  <si>
+    <t>End the Invoices loop</t>
+  </si>
+  <si>
+    <t>End the If any Invoices statement</t>
+  </si>
+  <si>
+    <t>End the If any Invoice Payment Requests statement</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>InvoiceDate</t>
+  </si>
+  <si>
+    <t>TotalPaymentAmount</t>
+  </si>
+  <si>
+    <t>MatchAmount</t>
+  </si>
+  <si>
+    <t>GrantNumber</t>
+  </si>
+  <si>
+    <t>ProgramIndexCode</t>
+  </si>
+  <si>
+    <t>ProjectCodeName</t>
+  </si>
+  <si>
+    <t>OrganizationCodeName</t>
+  </si>
+  <si>
+    <t>InvoiceNumber</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>Appn</t>
+  </si>
+  <si>
+    <t>SubObject</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.InvoiceDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.TotalPaymentAmount %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.MatchAmount %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.GrantNumber %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.ProgramIndexCode %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.ProjectCodeName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.OrganizationCodeName %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.InvoiceNumber %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.Fund %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.Appn %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.SubObject %&gt;</t>
   </si>
 </sst>
 </file>
@@ -1538,23 +1762,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="77.88671875" customWidth="1"/>
-    <col min="5" max="5" width="100.5546875" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.5703125" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1796,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>126</v>
       </c>
@@ -1586,7 +1810,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -1604,7 +1828,7 @@
       </c>
       <c r="F3" s="46"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="46" t="s">
         <v>12</v>
@@ -1618,7 +1842,7 @@
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51" t="s">
@@ -1632,7 +1856,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51" t="s">
@@ -1646,7 +1870,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51" t="s">
@@ -1660,7 +1884,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51" t="s">
@@ -1674,7 +1898,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51" t="s">
@@ -1688,7 +1912,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51" t="s">
@@ -1702,7 +1926,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51" t="s">
@@ -1716,7 +1940,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
@@ -1730,7 +1954,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51" t="s">
@@ -1744,7 +1968,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51" t="s">
@@ -1758,7 +1982,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51" t="s">
@@ -1772,7 +1996,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51" t="s">
@@ -1786,7 +2010,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51" t="s">
@@ -1800,7 +2024,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51" t="s">
@@ -1814,7 +2038,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
@@ -1830,7 +2054,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51" t="s">
@@ -1846,7 +2070,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
         <v>223</v>
       </c>
@@ -1866,7 +2090,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
         <v>224</v>
       </c>
@@ -1886,7 +2110,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="51" t="s">
         <v>121</v>
       </c>
@@ -1906,7 +2130,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>118</v>
       </c>
@@ -1926,7 +2150,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>129</v>
       </c>
@@ -1946,7 +2170,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>152</v>
       </c>
@@ -1966,7 +2190,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>152</v>
       </c>
@@ -1986,19 +2210,379 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="F28" s="51" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C29" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D29" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="37"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="37"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2010,20 +2594,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B737C5F2-D331-4EC0-AE50-ADE7E7050ACA}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2038,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2053,7 +2637,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2066,7 +2650,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>152</v>
       </c>
@@ -2083,7 +2667,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -2096,7 +2680,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -2109,7 +2693,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>129</v>
       </c>
@@ -2122,7 +2706,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -2133,7 +2717,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -2144,7 +2728,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -2157,7 +2741,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -2170,7 +2754,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -2183,7 +2767,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -2196,7 +2780,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -2209,7 +2793,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>152</v>
       </c>
@@ -2226,7 +2810,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
@@ -2239,7 +2823,7 @@
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
@@ -2252,7 +2836,7 @@
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>129</v>
       </c>
@@ -2265,7 +2849,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
@@ -2276,7 +2860,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
@@ -2287,7 +2871,7 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
@@ -2300,7 +2884,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
@@ -2313,7 +2897,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
@@ -2326,7 +2910,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
         <v>40</v>
@@ -2339,7 +2923,7 @@
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
@@ -2352,7 +2936,7 @@
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>129</v>
       </c>
@@ -2369,7 +2953,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
@@ -2382,7 +2966,7 @@
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>129</v>
       </c>
@@ -2395,7 +2979,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
@@ -2406,7 +2990,7 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
@@ -2417,7 +3001,7 @@
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
@@ -2430,7 +3014,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
@@ -2443,7 +3027,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
@@ -2456,7 +3040,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
         <v>40</v>
@@ -2480,19 +3064,19 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2507,7 +3091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +3108,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2537,7 +3121,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>118</v>
       </c>
@@ -2554,7 +3138,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -2567,7 +3151,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -2580,7 +3164,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>114</v>
       </c>
@@ -2593,7 +3177,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -2604,7 +3188,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -2615,7 +3199,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -2626,7 +3210,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -2637,7 +3221,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
@@ -2652,7 +3236,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -2667,7 +3251,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -2680,7 +3264,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -2693,7 +3277,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -2716,19 +3300,19 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2743,7 +3327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
@@ -2758,7 +3342,7 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
@@ -2771,7 +3355,7 @@
       </c>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>121</v>
       </c>
@@ -2788,7 +3372,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -2801,7 +3385,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -2814,7 +3398,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>183</v>
       </c>
@@ -2827,7 +3411,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -2838,7 +3422,7 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -2849,7 +3433,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -2860,7 +3444,7 @@
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -2871,7 +3455,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
@@ -2882,7 +3466,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="24" t="s">
         <v>5</v>
@@ -2897,7 +3481,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -2910,7 +3494,7 @@
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -2921,7 +3505,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -2948,16 +3532,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2972,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2987,7 +3571,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3000,7 +3584,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>114</v>
       </c>
@@ -3017,7 +3601,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3030,7 +3614,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3043,7 +3627,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>99</v>
       </c>
@@ -3060,7 +3644,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3071,7 +3655,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3082,7 +3666,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3093,7 +3677,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3104,7 +3688,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3115,7 +3699,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -3130,7 +3714,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>40</v>
@@ -3143,7 +3727,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>7</v>
@@ -3156,7 +3740,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -3182,16 +3766,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3206,7 +3790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3221,7 +3805,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3234,7 +3818,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>121</v>
       </c>
@@ -3251,7 +3835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3264,7 +3848,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3277,7 +3861,7 @@
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>98</v>
       </c>
@@ -3294,7 +3878,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -3305,7 +3889,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -3316,7 +3900,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -3327,7 +3911,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -3338,7 +3922,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
@@ -3353,7 +3937,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -3366,7 +3950,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -3379,7 +3963,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -3392,7 +3976,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -3418,16 +4002,16 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="55.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3442,7 +4026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -3459,7 +4043,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3472,7 +4056,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>223</v>
       </c>
@@ -3489,7 +4073,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3502,7 +4086,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3515,7 +4099,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>206</v>
       </c>
@@ -3528,7 +4112,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3539,7 +4123,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3550,7 +4134,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3561,7 +4145,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3572,7 +4156,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3583,7 +4167,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -3596,7 +4180,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -3609,7 +4193,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
         <v>40</v>
@@ -3635,16 +4219,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="92.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3659,7 +4243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -3676,7 +4260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3689,7 +4273,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>224</v>
       </c>
@@ -3706,7 +4290,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3719,7 +4303,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3732,7 +4316,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>212</v>
       </c>
@@ -3745,7 +4329,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3756,7 +4340,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3769,7 +4353,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3782,7 +4366,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3793,7 +4377,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>40</v>
@@ -3806,7 +4390,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
@@ -3819,7 +4403,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
         <v>40</v>
@@ -3836,4 +4420,311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WADNR-2004 Add existing WADNR fields to report generator - Filled out models and added (hopefully) useful properties - Updated documentation spreadsheet
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\wadnrforesthealth\Source\ProjectFirma.Web\Content\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74906FC8-FC48-404A-9898-712FAA7B14A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC30CF-D810-49A3-B8B6-704933F92976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="642" activeTab="9" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,11 @@
     <sheet name="Organization" sheetId="3" r:id="rId6"/>
     <sheet name="ReportedPerformanceMeasure" sheetId="8" r:id="rId7"/>
     <sheet name="ExpectedPerformanceMeasure" sheetId="9" r:id="rId8"/>
-    <sheet name="InvoicePaymentRequest" sheetId="10" r:id="rId9"/>
-    <sheet name="Invoice" sheetId="12" r:id="rId10"/>
+    <sheet name="ProjectRegion" sheetId="15" r:id="rId9"/>
+    <sheet name="ProjectCounty" sheetId="14" r:id="rId10"/>
+    <sheet name="ProjectTreatment" sheetId="16" r:id="rId11"/>
+    <sheet name="InvoicePaymentRequest" sheetId="10" r:id="rId12"/>
+    <sheet name="Invoice" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="392">
   <si>
     <t>Description of Field</t>
   </si>
@@ -320,16 +323,10 @@
     <t>Project Contact Names</t>
   </si>
   <si>
-    <t xml:space="preserve">Returns a comma delimited list of contacts that belong to the contact type entered. </t>
-  </si>
-  <si>
     <t>Project Organization Names</t>
   </si>
   <si>
     <t>&lt;%= project.GetProjectOrganizationNamesByType("Funder") %&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Returns a comma delimited list of organizations that belong to the organization type entered. </t>
   </si>
   <si>
     <t>&lt;%= project.GetProjectContactNamesByType("Project Manager") %&gt;</t>
@@ -926,12 +923,6 @@
     <t>Get All Project Expected Performance Measure values</t>
   </si>
   <si>
-    <t>Tenant Specificity</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Entering subcategory information is optional for Expected Performance Measures, so this may return an empty string</t>
   </si>
   <si>
@@ -953,9 +944,6 @@
     <t>Returns a list of InvoicePaymentRequest models (see InvoicePaymentRequest tab)</t>
   </si>
   <si>
-    <t>WADNR</t>
-  </si>
-  <si>
     <t>InvoicePaymentRequests</t>
   </si>
   <si>
@@ -1167,6 +1155,339 @@
   </si>
   <si>
     <t>&lt;%= invoice.SubObject %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% var reportedPerformanceMeasures = project.GetProjectReportedPerformanceMeasures(); %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% var expectedPerformanceMeasures = project.GetProjectExpectedPerformanceMeasures(); %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.PercentageMatch %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.PercentageMatchDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ProjectLastUpdatedDisplay %&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval Date </t>
+  </si>
+  <si>
+    <t>Project Last Updated Formatted to MM/DD/YYYY</t>
+  </si>
+  <si>
+    <t>Percentage Match for Treatment Costs</t>
+  </si>
+  <si>
+    <t>Percentage Match With a Percent Sign</t>
+  </si>
+  <si>
+    <t>Expiration Date</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ApprovalDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ApprovalDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ExpirationDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ExpirationDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>Project County(s)</t>
+  </si>
+  <si>
+    <t>Approval Date Formatted</t>
+  </si>
+  <si>
+    <t>Expiration Date Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ProjectCountiesDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>Returns a comma-delimited list of counties that the project is located in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returns a comma-delimited list of organizations that belong to the organization type entered. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returns a comma-delimited list of contacts that belong to the contact type entered. </t>
+  </si>
+  <si>
+    <t>Formatted to MM/DD/YYYY</t>
+  </si>
+  <si>
+    <t>ProjectCounty(s)</t>
+  </si>
+  <si>
+    <t>Get all Project Counties</t>
+  </si>
+  <si>
+    <t>ProjectRegion(s)</t>
+  </si>
+  <si>
+    <t>Get all Project Regions</t>
+  </si>
+  <si>
+    <t>ProjectTreatment(s)</t>
+  </si>
+  <si>
+    <t>Get all Project Treatments</t>
+  </si>
+  <si>
+    <t>Project Region(s)</t>
+  </si>
+  <si>
+    <t>&lt;%= project.ProjectRegionsDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>Returns a comma-delimited list of regions that the project is located in.</t>
+  </si>
+  <si>
+    <t>&lt;% var regions = project.GetProjectRegions(); %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% var treatments = project.GetProjectTreatments(); %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% var counties = project.GetProjectCounties(); %&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectRegion models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ProjectRegion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectCounty models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ProjectCounty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of ProjectTreatment models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ProjectTreatment </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tab)</t>
+    </r>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>&lt;%= projectContact.Address %&gt;</t>
+  </si>
+  <si>
+    <t>Get All Project Regions</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectRegion models</t>
+  </si>
+  <si>
+    <t>&lt;% if(regions.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>If there are Project Regions</t>
+  </si>
+  <si>
+    <t>Start Project Region loop</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var region in regions) { %&gt;</t>
+  </si>
+  <si>
+    <t>ProjectRegion</t>
+  </si>
+  <si>
+    <t>Region Name</t>
+  </si>
+  <si>
+    <t>Region Abbreviation</t>
+  </si>
+  <si>
+    <t>&lt;%= region.Abbreviation %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.Name %&gt;</t>
+  </si>
+  <si>
+    <t>Not all DNR Upland Regions have abbrevations</t>
+  </si>
+  <si>
+    <t>End the Project Region loop</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectCounty models</t>
+  </si>
+  <si>
+    <t>Start Project County loop</t>
+  </si>
+  <si>
+    <t>ProjectCounty</t>
+  </si>
+  <si>
+    <t>County Name</t>
+  </si>
+  <si>
+    <t>End the Project County loop</t>
+  </si>
+  <si>
+    <t>Get All Project Counties</t>
+  </si>
+  <si>
+    <t>If there are Project Counties</t>
+  </si>
+  <si>
+    <t>&lt;% if(counties.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var county in Countys) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= county.Name %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% if(treatments.Any()) { ?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;% foreach(var treatment in treatments) { %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.Name %&gt;</t>
+  </si>
+  <si>
+    <t>Get All Project Treatments</t>
+  </si>
+  <si>
+    <t>Returns a list of ProjectTreatment models</t>
+  </si>
+  <si>
+    <t>If there are Project Treatments</t>
+  </si>
+  <si>
+    <t>Start Project Treatment loop</t>
+  </si>
+  <si>
+    <t>ProjectTreatment</t>
+  </si>
+  <si>
+    <t>Treatment Name</t>
+  </si>
+  <si>
+    <t>End the Project Treatment loop</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.StartDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.StartDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>Start Date Formatted</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>End Date Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.EndDate %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.EndDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>Footprint Acres</t>
+  </si>
+  <si>
+    <t>Treated Acres</t>
+  </si>
+  <si>
+    <t>Cost Per Acre</t>
+  </si>
+  <si>
+    <t>Total Cost for Footprint Acres</t>
+  </si>
+  <si>
+    <t>Total Cost for Treated Acres</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.FootprintAcres %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TreatedAcres %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.CostPerAcre %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TotalCostFootprint %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TotalCostTreated %&gt;</t>
   </si>
 </sst>
 </file>
@@ -1762,23 +2083,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="100.5703125" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" customWidth="1"/>
+    <col min="5" max="5" width="100.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1792,25 +2110,21 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -1824,11 +2138,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="46"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="46"/>
       <c r="B4" s="46" t="s">
         <v>12</v>
@@ -1840,9 +2153,8 @@
         <v>13</v>
       </c>
       <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="51"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51" t="s">
@@ -1852,11 +2164,8 @@
         <v>15</v>
       </c>
       <c r="E5" s="51"/>
-      <c r="F5" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51" t="s">
@@ -1866,11 +2175,8 @@
         <v>43</v>
       </c>
       <c r="E6" s="51"/>
-      <c r="F6" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51" t="s">
@@ -1880,11 +2186,8 @@
         <v>16</v>
       </c>
       <c r="E7" s="51"/>
-      <c r="F7" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51" t="s">
@@ -1894,11 +2197,8 @@
         <v>19</v>
       </c>
       <c r="E8" s="51"/>
-      <c r="F8" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51" t="s">
@@ -1908,11 +2208,8 @@
         <v>21</v>
       </c>
       <c r="E9" s="51"/>
-      <c r="F9" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51" t="s">
@@ -1922,11 +2219,8 @@
         <v>23</v>
       </c>
       <c r="E10" s="51"/>
-      <c r="F10" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51" t="s">
@@ -1936,11 +2230,8 @@
         <v>32</v>
       </c>
       <c r="E11" s="51"/>
-      <c r="F11" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
@@ -1950,11 +2241,8 @@
         <v>36</v>
       </c>
       <c r="E12" s="51"/>
-      <c r="F12" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51" t="s">
@@ -1964,11 +2252,8 @@
         <v>33</v>
       </c>
       <c r="E13" s="51"/>
-      <c r="F13" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51" t="s">
@@ -1978,11 +2263,8 @@
         <v>37</v>
       </c>
       <c r="E14" s="51"/>
-      <c r="F14" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51" t="s">
@@ -1992,11 +2274,8 @@
         <v>38</v>
       </c>
       <c r="E15" s="51"/>
-      <c r="F15" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51" t="s">
@@ -2006,11 +2285,8 @@
         <v>34</v>
       </c>
       <c r="E16" s="51"/>
-      <c r="F16" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51" t="s">
@@ -2020,11 +2296,8 @@
         <v>39</v>
       </c>
       <c r="E17" s="51"/>
-      <c r="F17" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51" t="s">
@@ -2034,215 +2307,341 @@
         <v>35</v>
       </c>
       <c r="E18" s="51"/>
-      <c r="F18" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
-        <v>91</v>
+        <v>308</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>96</v>
+        <v>306</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51" t="s">
+        <v>309</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>304</v>
+      </c>
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21" s="51"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51" t="s">
+        <v>307</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="E22" s="51"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" s="51" t="s">
+        <v>313</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>314</v>
+      </c>
+      <c r="E24" s="51"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
+      <c r="E27" s="51" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="51"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51" t="s">
+        <v>330</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>331</v>
+      </c>
+      <c r="E28" s="51" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="E29" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>302</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="D31" s="51" t="s">
+        <v>303</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="51" t="s">
-        <v>184</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="E21" s="51" t="s">
-        <v>204</v>
-      </c>
-      <c r="F21" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="51" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="51" t="s">
+      <c r="C32" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="D22" s="51" t="s">
-        <v>203</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="F22" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="51" t="s">
+      <c r="C33" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="54" t="s">
+      <c r="C34" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="C35" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="D35" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="52" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="55" t="s">
+      <c r="C36" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="55" t="s">
+      <c r="E36" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="B37" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="55" t="s">
+      <c r="C37" s="55" t="s">
+        <v>327</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="B38" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="C38" s="55" t="s">
+        <v>325</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="55" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="55" t="s">
+        <v>329</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>334</v>
+      </c>
+      <c r="E39" s="55" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="D40" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="B28" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>237</v>
-      </c>
-      <c r="D28" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>234</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47" t="s">
+      <c r="E40" s="55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C41" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D41" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
+      <c r="E41" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2251,23 +2650,751 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4A8308-54D6-46DD-9EA5-2A41604CB106}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
+      <c r="B10" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4D27C8-0D89-4003-B55E-37B1C4839260}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" s="51"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="E12" s="51"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="E13" s="51"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="E14" s="51"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="E15" s="51"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="E16" s="51"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
+      <c r="B19" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="41"/>
+      <c r="B23" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2282,7 +3409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2297,7 +3424,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2310,268 +3437,268 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="37"/>
       <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
       <c r="B9" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>279</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="E9" s="37"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>284</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="37"/>
       <c r="B21" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D21" s="37" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="37"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D22" s="37" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="37"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
       <c r="B25" s="43" t="s">
         <v>40</v>
@@ -2594,20 +3721,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B737C5F2-D331-4EC0-AE50-ADE7E7050ACA}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2622,7 +3747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -2637,7 +3762,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2650,397 +3775,397 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
         <v>40</v>
@@ -3063,20 +4188,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FB6253-126F-48A7-BD83-7AF928C5064F}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3091,7 +4214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -3105,10 +4228,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3121,9 +4244,9 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
@@ -3138,7 +4261,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3151,7 +4274,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3164,9 +4287,9 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
@@ -3177,7 +4300,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3188,7 +4311,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3199,7 +4322,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3210,7 +4333,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3221,7 +4344,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
@@ -3236,7 +4359,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -3251,7 +4374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -3264,7 +4387,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -3277,7 +4400,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -3297,22 +4420,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9A6D10-D005-4028-9B06-C7C6D4527AEB}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -3327,7 +4448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
@@ -3342,7 +4463,7 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
@@ -3355,9 +4476,9 @@
       </c>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>5</v>
@@ -3369,10 +4490,10 @@
         <v>45</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -3385,7 +4506,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -3398,9 +4519,9 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24" t="s">
@@ -3411,7 +4532,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -3422,7 +4543,7 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -3433,7 +4554,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -3444,7 +4565,7 @@
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -3455,68 +4576,79 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D13" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24" t="s">
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="24" t="s">
+      <c r="C14" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="D15" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="43" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
+      <c r="B17" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C17" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E17" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3526,22 +4658,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FA0FB6-A69B-47A6-B1F1-D75B486891E8}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3556,7 +4686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3571,7 +4701,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3584,9 +4714,9 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -3601,7 +4731,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3614,7 +4744,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3627,9 +4757,9 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>5</v>
@@ -3644,114 +4774,125 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="43" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
+      <c r="B17" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C17" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="44"/>
+      <c r="E17" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3762,20 +4903,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5965BDDB-E97D-4E2A-8C75-63D76FB39378}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3790,7 +4929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3805,7 +4944,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3818,9 +4957,9 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
@@ -3832,10 +4971,10 @@
         <v>45</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3848,28 +4987,28 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>88</v>
@@ -3878,66 +5017,66 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
         <v>69</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
         <v>73</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>115</v>
-      </c>
       <c r="E12" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -3950,7 +5089,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -3963,7 +5102,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -3976,7 +5115,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -3998,20 +5137,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345078EF-4E02-4B0D-B586-01D7A19E1A69}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4026,7 +5163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4040,10 +5177,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4056,131 +5193,131 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -4193,7 +5330,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
         <v>40</v>
@@ -4215,20 +5352,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4243,7 +5378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4257,10 +5392,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4273,124 +5408,124 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
@@ -4403,7 +5538,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
         <v>40</v>
@@ -4423,39 +5558,37 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B2124-FD35-456C-8F21-FC7C1773932E}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="39" t="s">
@@ -4467,9 +5600,11 @@
       <c r="D2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="40"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4482,249 +5617,116 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
+      <c r="C4" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>244</v>
+      <c r="C6" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>347</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>245</v>
+        <v>349</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>246</v>
+        <v>348</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>261</v>
+        <v>351</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="E16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C9" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="43" t="s">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C11" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D11" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E11" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WADNR-2005 Add Invoices section to Project Detail page update Report Generator docs with correct Invoice field fix bug with modals ensure Org Code is saved
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\wadnrforesthealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC30CF-D810-49A3-B8B6-704933F92976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7BEC4-78BE-4C5D-B974-33DB702BD7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="642" firstSheet="2" activeTab="12" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1094,9 +1094,6 @@
     <t>InvoiceDate</t>
   </si>
   <si>
-    <t>TotalPaymentAmount</t>
-  </si>
-  <si>
     <t>MatchAmount</t>
   </si>
   <si>
@@ -1125,9 +1122,6 @@
   </si>
   <si>
     <t>&lt;%= invoice.InvoiceDate %&gt;</t>
-  </si>
-  <si>
-    <t>&lt;%= invoice.TotalPaymentAmount %&gt;</t>
   </si>
   <si>
     <t>&lt;%= invoice.MatchAmount %&gt;</t>
@@ -1488,6 +1482,12 @@
   </si>
   <si>
     <t>&lt;%= treatment.TotalCostTreated %&gt;</t>
+  </si>
+  <si>
+    <t>PaymentAmount</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.PaymentAmount %&gt;</t>
   </si>
 </sst>
 </file>
@@ -2085,18 +2085,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="77.88671875" customWidth="1"/>
-    <col min="5" max="5" width="100.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>124</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="46" t="s">
         <v>12</v>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="E4" s="46"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51" t="s">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51" t="s">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51" t="s">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="E7" s="51"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51" t="s">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="E8" s="51"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51" t="s">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="E9" s="51"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51" t="s">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="E10" s="51"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51" t="s">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="E11" s="51"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="E12" s="51"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51" t="s">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51" t="s">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="E14" s="51"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51" t="s">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51" t="s">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="E16" s="51"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51" t="s">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51" t="s">
@@ -2308,90 +2308,90 @@
       </c>
       <c r="E18" s="51"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E20" s="51"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E21" s="51"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E22" s="51"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E24" s="51"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51" t="s">
@@ -2401,10 +2401,10 @@
         <v>94</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51" t="s">
@@ -2414,36 +2414,36 @@
         <v>93</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="51" t="s">
+        <v>329</v>
+      </c>
+      <c r="E28" s="51" t="s">
         <v>330</v>
       </c>
-      <c r="D28" s="51" t="s">
-        <v>331</v>
-      </c>
-      <c r="E28" s="51" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
         <v>221</v>
       </c>
@@ -2454,13 +2454,13 @@
         <v>182</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
         <v>222</v>
       </c>
@@ -2471,13 +2471,13 @@
         <v>223</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E31" s="51" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
         <v>119</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>116</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
         <v>127</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>150</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="53" t="s">
         <v>150</v>
       </c>
@@ -2562,58 +2562,58 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B37" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B38" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D38" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="E38" s="55" t="s">
         <v>335</v>
       </c>
-      <c r="E38" s="55" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="53" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B39" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
         <v>229</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="47" t="s">
         <v>40</v>
@@ -2655,16 +2655,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="92.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2709,76 +2709,76 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>7</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="41"/>
       <c r="B10" s="43" t="s">
         <v>40</v>
@@ -2816,16 +2816,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2870,179 +2870,179 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>380</v>
-      </c>
       <c r="E10" s="51"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>381</v>
-      </c>
       <c r="E11" s="51" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E12" s="51"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E14" s="51"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E16" s="51"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
         <v>7</v>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="43" t="s">
         <v>40</v>
@@ -3080,16 +3080,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>239</v>
       </c>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3243,7 +3243,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="23" t="s">
         <v>5</v>
@@ -3335,7 +3335,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>40</v>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
         <v>7</v>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="43" t="s">
         <v>40</v>
@@ -3383,18 +3383,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3409,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3424,7 +3426,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3437,7 +3439,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3467,7 +3469,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3480,7 +3482,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>253</v>
       </c>
@@ -3497,7 +3499,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="32" t="s">
         <v>6</v>
@@ -3510,7 +3512,7 @@
       </c>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="32" t="s">
         <v>12</v>
@@ -3523,7 +3525,7 @@
       </c>
       <c r="E9" s="37"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>279</v>
       </c>
@@ -3532,121 +3534,121 @@
         <v>280</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>281</v>
+        <v>390</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>292</v>
+        <v>391</v>
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="37" t="s">
         <v>40</v>
@@ -3659,7 +3661,7 @@
       </c>
       <c r="E21" s="37"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="37" t="s">
         <v>7</v>
@@ -3672,7 +3674,7 @@
       </c>
       <c r="E22" s="37"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
         <v>40</v>
@@ -3685,7 +3687,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
         <v>7</v>
@@ -3698,7 +3700,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
       <c r="B25" s="43" t="s">
         <v>40</v>
@@ -3723,16 +3725,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3747,7 +3749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3762,7 +3764,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3775,7 +3777,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>150</v>
       </c>
@@ -3792,7 +3794,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3805,7 +3807,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3818,7 +3820,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>127</v>
       </c>
@@ -3831,7 +3833,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3842,7 +3844,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3853,7 +3855,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3866,7 +3868,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3879,7 +3881,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3892,7 +3894,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -3905,7 +3907,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -3918,7 +3920,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>150</v>
       </c>
@@ -3935,7 +3937,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
@@ -3948,7 +3950,7 @@
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
@@ -3961,7 +3963,7 @@
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>127</v>
       </c>
@@ -3974,7 +3976,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
@@ -3985,7 +3987,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
@@ -3996,7 +3998,7 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
@@ -4009,7 +4011,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
@@ -4022,7 +4024,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
@@ -4035,7 +4037,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
         <v>40</v>
@@ -4048,7 +4050,7 @@
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
@@ -4061,7 +4063,7 @@
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>127</v>
       </c>
@@ -4078,7 +4080,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
@@ -4091,7 +4093,7 @@
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>127</v>
       </c>
@@ -4104,7 +4106,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
@@ -4115,7 +4117,7 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
@@ -4126,7 +4128,7 @@
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
@@ -4139,7 +4141,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
@@ -4152,7 +4154,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
@@ -4165,7 +4167,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
         <v>40</v>
@@ -4190,16 +4192,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4214,7 +4216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4244,7 +4246,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>116</v>
       </c>
@@ -4261,7 +4263,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4274,7 +4276,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4287,7 +4289,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>112</v>
       </c>
@@ -4300,7 +4302,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4311,7 +4313,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4322,7 +4324,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4333,7 +4335,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4344,7 +4346,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
@@ -4359,7 +4361,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -4374,7 +4376,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -4387,7 +4389,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -4400,7 +4402,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -4424,16 +4426,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4448,7 +4450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
@@ -4463,7 +4465,7 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
@@ -4476,7 +4478,7 @@
       </c>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>119</v>
       </c>
@@ -4493,7 +4495,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -4506,7 +4508,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -4519,7 +4521,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>181</v>
       </c>
@@ -4532,7 +4534,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -4543,7 +4545,7 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -4554,7 +4556,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -4565,7 +4567,7 @@
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -4576,18 +4578,18 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
@@ -4598,7 +4600,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="24" t="s">
         <v>5</v>
@@ -4613,7 +4615,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>40</v>
@@ -4626,7 +4628,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="11" t="s">
         <v>7</v>
@@ -4637,7 +4639,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="43" t="s">
         <v>40</v>
@@ -4662,16 +4664,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4686,7 +4688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -4701,7 +4703,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4714,7 +4716,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>112</v>
       </c>
@@ -4731,7 +4733,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -4744,7 +4746,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -4757,7 +4759,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>97</v>
       </c>
@@ -4774,7 +4776,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4785,7 +4787,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4796,7 +4798,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4807,7 +4809,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4818,7 +4820,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -4829,18 +4831,18 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23" t="s">
         <v>5</v>
@@ -4855,7 +4857,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>40</v>
@@ -4868,7 +4870,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>7</v>
@@ -4881,7 +4883,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="43" t="s">
         <v>40</v>
@@ -4905,16 +4907,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4929,7 +4931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -4944,7 +4946,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4957,7 +4959,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>119</v>
       </c>
@@ -4974,7 +4976,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4987,7 +4989,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5000,7 +5002,7 @@
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>96</v>
       </c>
@@ -5017,7 +5019,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -5028,7 +5030,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -5039,7 +5041,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -5050,7 +5052,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -5061,7 +5063,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
@@ -5076,7 +5078,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -5089,7 +5091,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -5102,7 +5104,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -5115,7 +5117,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -5139,16 +5141,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="55.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5180,7 +5182,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5193,7 +5195,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>221</v>
       </c>
@@ -5210,7 +5212,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5223,7 +5225,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5236,7 +5238,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>204</v>
       </c>
@@ -5249,7 +5251,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5260,7 +5262,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5271,7 +5273,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5282,7 +5284,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5293,7 +5295,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -5304,7 +5306,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -5317,7 +5319,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -5330,7 +5332,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
         <v>40</v>
@@ -5354,16 +5356,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="92.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5378,7 +5380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5395,7 +5397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5408,7 +5410,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>222</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5438,7 +5440,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5451,7 +5453,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>210</v>
       </c>
@@ -5464,7 +5466,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5475,7 +5477,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5488,7 +5490,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5501,7 +5503,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5512,7 +5514,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>40</v>
@@ -5525,7 +5527,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
@@ -5538,7 +5540,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
         <v>40</v>
@@ -5563,16 +5565,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" customWidth="1"/>
-    <col min="4" max="4" width="78.5546875" customWidth="1"/>
-    <col min="5" max="5" width="92.5546875" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5587,7 +5589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5604,7 +5606,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5617,89 +5619,89 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>345</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>347</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D7" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>350</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>7</v>
@@ -5712,7 +5714,7 @@
       </c>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="43" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
WADNR-1989 Add IPR and Invoice fields to report generator - Added -Display properties of DateTime and Decimal (and nullable versions) to report properties for use in templates - Added VendorAddressDisplay to concatenate address components - Updated documentation for changes
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\wadnrforesthealth\Source\ProjectFirma.Web\Content\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7BEC4-78BE-4C5D-B974-33DB702BD7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12408F50-9E47-4C9A-92AF-559BC93F3CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="642" firstSheet="2" activeTab="12" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="36570" yWindow="7245" windowWidth="43200" windowHeight="23535" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="414">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1488,6 +1488,72 @@
   </si>
   <si>
     <t>&lt;%= invoice.PaymentAmount %&gt;</t>
+  </si>
+  <si>
+    <t>PaymentAmountDisplay</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.PaymentAmountDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>MatchAmountDisplay</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.MatchAmountDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Display as currency with X decimal places, rounded. If X is not provided, the default is 2, e.g. $123.45</t>
+  </si>
+  <si>
+    <t>VendorAddressDisplay</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorAddressDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>VendorCityStateZip</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.VendorCityStateZip %&gt;</t>
+  </si>
+  <si>
+    <t>Combines city, state, and ZIP in a standard template; empty components are not shown</t>
+  </si>
+  <si>
+    <t>Combines address lines and VendorCityStateZip in a standard template; empty components are not shown</t>
+  </si>
+  <si>
+    <t>Footprint Acres Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.FootprintAcresDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Treated Acres Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TreatedAcresDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Display with X decimal places, rounded. If X is not provided, the default is 3, e.g. 12.345</t>
+  </si>
+  <si>
+    <t>Cost Per Acre Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.CostPerAcreDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Total Cost for Treated Acres Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TotalCostTreatedDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Total Cost for Footprint Acres Formatted</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.TotalCostFootprintDisplay(X) %&gt;</t>
   </si>
 </sst>
 </file>
@@ -2085,7 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2096,7 +2162,7 @@
     <col min="5" max="5" width="100.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2812,7 +2878,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4D27C8-0D89-4003-B55E-37B1C4839260}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2822,7 +2888,7 @@
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2989,21 +3055,23 @@
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="E13" s="51"/>
+        <v>404</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E14" s="51"/>
     </row>
@@ -3011,62 +3079,125 @@
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>388</v>
-      </c>
-      <c r="E15" s="51"/>
+        <v>406</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="E16" s="51"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="E18" s="51"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D20" s="24" t="s">
         <v>389</v>
       </c>
-      <c r="E16" s="51"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11" t="s">
+      <c r="E20" s="51"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11" t="s">
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="43" t="s">
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C24" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D24" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="44"/>
+      <c r="E24" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3076,7 +3207,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3086,7 +3217,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" customWidth="1"/>
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3269,32 +3400,36 @@
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>248</v>
+        <v>399</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="E15" s="25"/>
+        <v>400</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>249</v>
+        <v>397</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E16" s="25"/>
+        <v>398</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E17" s="25"/>
     </row>
@@ -3302,10 +3437,10 @@
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E18" s="25"/>
     </row>
@@ -3313,66 +3448,88 @@
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E21" s="25"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C22" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E22" s="25" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="43" t="s">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C25" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D25" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E25" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3381,11 +3538,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3393,7 +3548,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" customWidth="1"/>
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3553,21 +3708,23 @@
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>281</v>
+        <v>392</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="E12" s="25"/>
+        <v>393</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E13" s="25"/>
     </row>
@@ -3575,21 +3732,23 @@
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>283</v>
+        <v>394</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="E14" s="25"/>
+        <v>395</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E15" s="25"/>
     </row>
@@ -3597,10 +3756,10 @@
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E16" s="25"/>
     </row>
@@ -3608,10 +3767,10 @@
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E17" s="25"/>
     </row>
@@ -3619,10 +3778,10 @@
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E18" s="25"/>
     </row>
@@ -3630,10 +3789,10 @@
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E19" s="25"/>
     </row>
@@ -3641,77 +3800,99 @@
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" s="25"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37" t="s">
+      <c r="E22" s="25"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C23" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D23" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="37"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37" t="s">
+      <c r="E23" s="37"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+      <c r="B24" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C24" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D24" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="37"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="E24" s="37"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="43" t="s">
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C27" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D27" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="44"/>
+      <c r="E27" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4424,7 +4605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9A6D10-D005-4028-9B06-C7C6D4527AEB}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4435,7 +4618,7 @@
     <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
WADNR-2004 Add existing WADNR fields to report generator - Expanded Report Region per Dan's feedback - Added TreatmentCode back in - Updated documentation for changes
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12408F50-9E47-4C9A-92AF-559BC93F3CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DDAE71-1F50-4EC4-8DA2-EC03B16D1B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36570" yWindow="7245" windowWidth="43200" windowHeight="23535" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="10905" yWindow="2730" windowWidth="38370" windowHeight="23370" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="431">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1055,9 +1055,6 @@
     <t>&lt;%= invoicePaymentRequest.Notes %&gt;</t>
   </si>
   <si>
-    <t>Returns a list of Invoice models (see invoice tab)</t>
-  </si>
-  <si>
     <t>&lt;% var invoices = invoicePaymentRequest.GetInvoices(); %&gt;</t>
   </si>
   <si>
@@ -1554,6 +1551,80 @@
   </si>
   <si>
     <t>&lt;%= treatment.TotalCostFootprintDisplay(X) %&gt;</t>
+  </si>
+  <si>
+    <t>Treatment Code</t>
+  </si>
+  <si>
+    <t>&lt;%= treatment.Code %&gt;</t>
+  </si>
+  <si>
+    <t>Region Address</t>
+  </si>
+  <si>
+    <t>Region City</t>
+  </si>
+  <si>
+    <t>Region State</t>
+  </si>
+  <si>
+    <t>Region ZIP</t>
+  </si>
+  <si>
+    <t>Region Combined Address Formatted</t>
+  </si>
+  <si>
+    <t>Combines Address, City, State, and ZIP in a standard template</t>
+  </si>
+  <si>
+    <t>Region Email</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returns a list of Invoice models (see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Invoice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> tab)</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;%= region.Address %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.AddressDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.City %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.State %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.ZIP %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= region.Email %&gt;</t>
+  </si>
+  <si>
+    <t>Region Phone</t>
+  </si>
+  <si>
+    <t>&lt;%= region.Phone %&gt;</t>
   </si>
 </sst>
 </file>
@@ -2378,23 +2449,23 @@
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E20" s="51"/>
     </row>
@@ -2402,10 +2473,10 @@
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E21" s="51"/>
     </row>
@@ -2413,10 +2484,10 @@
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E22" s="51"/>
     </row>
@@ -2424,23 +2495,23 @@
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E24" s="51"/>
     </row>
@@ -2448,13 +2519,13 @@
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2467,7 +2538,7 @@
         <v>94</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2480,33 +2551,33 @@
         <v>93</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51" t="s">
+        <v>327</v>
+      </c>
+      <c r="D28" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="E28" s="51" t="s">
         <v>329</v>
-      </c>
-      <c r="E28" s="51" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D29" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="E29" s="51" t="s">
         <v>317</v>
-      </c>
-      <c r="E29" s="51" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2520,7 +2591,7 @@
         <v>182</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>202</v>
@@ -2537,7 +2608,7 @@
         <v>223</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E31" s="51" t="s">
         <v>203</v>
@@ -2630,53 +2701,53 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="53" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B37" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="53" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B38" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B39" s="55" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2777,19 +2848,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,10 +2869,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>358</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>359</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -2811,23 +2882,23 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -2837,7 +2908,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>42</v>
@@ -2878,7 +2949,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4D27C8-0D89-4003-B55E-37B1C4839260}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2938,19 +3009,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>365</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2959,10 +3030,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -2972,34 +3043,34 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>364</v>
+        <v>414</v>
       </c>
       <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -3007,179 +3078,177 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>374</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>321</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>378</v>
-      </c>
-      <c r="E10" s="51"/>
+        <v>373</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>379</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>321</v>
-      </c>
+      <c r="E11" s="51"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>385</v>
-      </c>
-      <c r="E12" s="51"/>
+        <v>378</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>404</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>407</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="E13" s="51"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="E14" s="51"/>
+        <v>403</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>405</v>
+        <v>380</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>406</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>407</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="E15" s="51"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>387</v>
-      </c>
-      <c r="E16" s="51"/>
+        <v>405</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>408</v>
+        <v>381</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>409</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>396</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="E17" s="51"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>383</v>
+        <v>407</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>388</v>
-      </c>
-      <c r="E18" s="51"/>
+        <v>408</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>413</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>396</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>384</v>
+        <v>411</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>389</v>
-      </c>
-      <c r="E20" s="51"/>
+        <v>412</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="E21" s="51"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>411</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="25" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>83</v>
+        <v>370</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>42</v>
@@ -3187,17 +3256,30 @@
       <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="43" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C25" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D25" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="44"/>
+      <c r="E25" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3217,7 +3299,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" customWidth="1"/>
     <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3400,26 +3482,26 @@
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="E15" s="25" t="s">
         <v>400</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="D16" s="24" t="s">
-        <v>398</v>
-      </c>
       <c r="E16" s="25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,10 +3568,10 @@
         <v>253</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="E22" s="25" t="s">
         <v>268</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3498,7 +3580,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>42</v>
@@ -3533,6 +3615,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3648,10 +3731,10 @@
         <v>253</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3660,10 +3743,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>271</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>272</v>
       </c>
       <c r="E8" s="37"/>
     </row>
@@ -3673,23 +3756,23 @@
         <v>12</v>
       </c>
       <c r="C9" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="D9" s="37" t="s">
         <v>274</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>275</v>
       </c>
       <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E10" s="25"/>
     </row>
@@ -3697,10 +3780,10 @@
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>390</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>391</v>
       </c>
       <c r="E11" s="25"/>
     </row>
@@ -3708,23 +3791,23 @@
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>393</v>
-      </c>
       <c r="E12" s="25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E13" s="25"/>
     </row>
@@ -3732,23 +3815,23 @@
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="E14" s="25" t="s">
         <v>395</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15" s="25"/>
     </row>
@@ -3756,10 +3839,10 @@
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="25"/>
     </row>
@@ -3767,10 +3850,10 @@
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E17" s="25"/>
     </row>
@@ -3778,10 +3861,10 @@
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E18" s="25"/>
     </row>
@@ -3789,10 +3872,10 @@
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E19" s="25"/>
     </row>
@@ -3800,10 +3883,10 @@
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E20" s="25"/>
     </row>
@@ -3811,10 +3894,10 @@
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21" s="25"/>
     </row>
@@ -3822,10 +3905,10 @@
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E22" s="25"/>
     </row>
@@ -3835,7 +3918,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>42</v>
@@ -3848,7 +3931,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>42</v>
@@ -3861,7 +3944,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>42</v>
@@ -3874,7 +3957,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>42</v>
@@ -4765,10 +4848,10 @@
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>337</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>338</v>
       </c>
       <c r="E12" s="24"/>
     </row>
@@ -5018,10 +5101,10 @@
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>337</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>338</v>
       </c>
       <c r="E13" s="24"/>
     </row>
@@ -5744,7 +5827,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5B2124-FD35-456C-8F21-FC7C1773932E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5804,19 +5887,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>339</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5825,10 +5908,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -5838,77 +5921,156 @@
         <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>348</v>
-      </c>
       <c r="E7" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>423</v>
+      </c>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>425</v>
+      </c>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>417</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24" t="s">
+        <v>418</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>427</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24" t="s">
+        <v>429</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>428</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C16" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="43" t="s">
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D18" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E18" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WADNR-1989 Add IPR and Invoice fields to report generator - Added InvoiceDateDisplay and InvoicePaymentRequestDateDisplay to the respective report models; missed them on the first pass. - Updated documentation for the two new values.
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DDAE71-1F50-4EC4-8DA2-EC03B16D1B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E16EC34-6099-4783-BAC6-A3F5DDB553DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="2730" windowWidth="38370" windowHeight="23370" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="5376" yWindow="5376" windowWidth="34560" windowHeight="18744" tabRatio="642" firstSheet="3" activeTab="11" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="435">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1625,6 +1625,18 @@
   </si>
   <si>
     <t>&lt;%= region.Phone %&gt;</t>
+  </si>
+  <si>
+    <t>InvoicePaymentRequestDateDisplay</t>
+  </si>
+  <si>
+    <t>&lt;%= invoicePaymentRequest.InvoicePaymentRequestDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.InvoiceDateDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>InvoiceDateDisplay</t>
   </si>
 </sst>
 </file>
@@ -2222,18 +2234,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="100.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" customWidth="1"/>
+    <col min="5" max="5" width="100.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2248,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="45" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>124</v>
       </c>
@@ -2261,7 +2273,7 @@
       </c>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="46"/>
       <c r="B4" s="46" t="s">
         <v>12</v>
@@ -2291,7 +2303,7 @@
       </c>
       <c r="E4" s="46"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="51"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51" t="s">
@@ -2302,7 +2314,7 @@
       </c>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51" t="s">
@@ -2313,7 +2325,7 @@
       </c>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51" t="s">
@@ -2324,7 +2336,7 @@
       </c>
       <c r="E7" s="51"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51" t="s">
@@ -2335,7 +2347,7 @@
       </c>
       <c r="E8" s="51"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51" t="s">
@@ -2346,7 +2358,7 @@
       </c>
       <c r="E9" s="51"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51" t="s">
@@ -2357,7 +2369,7 @@
       </c>
       <c r="E10" s="51"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51" t="s">
@@ -2368,7 +2380,7 @@
       </c>
       <c r="E11" s="51"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
@@ -2379,7 +2391,7 @@
       </c>
       <c r="E12" s="51"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51" t="s">
@@ -2390,7 +2402,7 @@
       </c>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51" t="s">
@@ -2401,7 +2413,7 @@
       </c>
       <c r="E14" s="51"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51" t="s">
@@ -2412,7 +2424,7 @@
       </c>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51" t="s">
@@ -2423,7 +2435,7 @@
       </c>
       <c r="E16" s="51"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51" t="s">
@@ -2434,7 +2446,7 @@
       </c>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51" t="s">
@@ -2445,7 +2457,7 @@
       </c>
       <c r="E18" s="51"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
@@ -2458,7 +2470,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51" t="s">
@@ -2469,7 +2481,7 @@
       </c>
       <c r="E20" s="51"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51" t="s">
@@ -2480,7 +2492,7 @@
       </c>
       <c r="E21" s="51"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51" t="s">
@@ -2491,7 +2503,7 @@
       </c>
       <c r="E22" s="51"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51" t="s">
@@ -2504,7 +2516,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51" t="s">
@@ -2515,7 +2527,7 @@
       </c>
       <c r="E24" s="51"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51" t="s">
@@ -2528,7 +2540,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51" t="s">
@@ -2541,7 +2553,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51" t="s">
@@ -2554,7 +2566,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51" t="s">
@@ -2567,7 +2579,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51" t="s">
@@ -2580,7 +2592,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="51" t="s">
         <v>221</v>
       </c>
@@ -2597,7 +2609,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="51" t="s">
         <v>222</v>
       </c>
@@ -2614,7 +2626,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="51" t="s">
         <v>119</v>
       </c>
@@ -2631,7 +2643,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>116</v>
       </c>
@@ -2648,7 +2660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="53" t="s">
         <v>127</v>
       </c>
@@ -2665,7 +2677,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="53" t="s">
         <v>150</v>
       </c>
@@ -2682,7 +2694,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="53" t="s">
         <v>150</v>
       </c>
@@ -2699,7 +2711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="53" t="s">
         <v>323</v>
       </c>
@@ -2716,7 +2728,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="53" t="s">
         <v>321</v>
       </c>
@@ -2733,7 +2745,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="53" t="s">
         <v>325</v>
       </c>
@@ -2750,7 +2762,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="53" t="s">
         <v>229</v>
       </c>
@@ -2767,7 +2779,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="47"/>
       <c r="B41" s="47" t="s">
         <v>40</v>
@@ -2792,16 +2804,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2816,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -2846,7 +2858,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>321</v>
       </c>
@@ -2863,7 +2875,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -2876,7 +2888,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -2889,7 +2901,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>353</v>
       </c>
@@ -2902,7 +2914,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>40</v>
@@ -2915,7 +2927,7 @@
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>7</v>
@@ -2928,7 +2940,7 @@
       </c>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="41"/>
       <c r="B10" s="43" t="s">
         <v>40</v>
@@ -2953,16 +2965,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -2977,7 +2989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3007,7 +3019,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>325</v>
       </c>
@@ -3024,7 +3036,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -3037,7 +3049,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -3050,7 +3062,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>368</v>
       </c>
@@ -3063,7 +3075,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3074,7 +3086,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3085,7 +3097,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3098,7 +3110,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3109,7 +3121,7 @@
       </c>
       <c r="E11" s="51"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3122,7 +3134,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
@@ -3133,7 +3145,7 @@
       </c>
       <c r="E13" s="51"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
@@ -3146,7 +3158,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
@@ -3157,7 +3169,7 @@
       </c>
       <c r="E15" s="51"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
@@ -3170,7 +3182,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
@@ -3181,7 +3193,7 @@
       </c>
       <c r="E17" s="51"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
@@ -3194,7 +3206,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
@@ -3205,7 +3217,7 @@
       </c>
       <c r="E19" s="51"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
@@ -3218,7 +3230,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
@@ -3229,7 +3241,7 @@
       </c>
       <c r="E21" s="51"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24" t="s">
@@ -3242,7 +3254,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>40</v>
@@ -3255,7 +3267,7 @@
       </c>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>7</v>
@@ -3268,7 +3280,7 @@
       </c>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
       <c r="B25" s="43" t="s">
         <v>40</v>
@@ -3289,20 +3301,20 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3332,7 +3344,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3345,7 +3357,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
@@ -3362,7 +3374,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3375,7 +3387,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3388,7 +3400,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>239</v>
       </c>
@@ -3401,7 +3413,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -3412,7 +3424,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -3423,7 +3435,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -3434,7 +3446,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -3445,7 +3457,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -3456,7 +3468,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
@@ -3467,7 +3479,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
@@ -3478,7 +3490,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
@@ -3491,7 +3503,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
@@ -3504,7 +3516,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
@@ -3515,7 +3527,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
@@ -3526,7 +3538,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
@@ -3537,7 +3549,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
@@ -3548,70 +3560,83 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23" t="s">
+      <c r="E22" s="25"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C23" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D23" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E23" s="31" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>83</v>
+        <v>269</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="43" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
+      <c r="B26" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C26" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D26" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="44"/>
+      <c r="E26" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3621,20 +3646,20 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3649,7 +3674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -3664,7 +3689,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -3677,7 +3702,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
@@ -3694,7 +3719,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -3707,7 +3732,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -3720,7 +3745,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>253</v>
       </c>
@@ -3737,7 +3762,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="37"/>
       <c r="B8" s="32" t="s">
         <v>6</v>
@@ -3750,7 +3775,7 @@
       </c>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
       <c r="B9" s="32" t="s">
         <v>12</v>
@@ -3763,7 +3788,7 @@
       </c>
       <c r="E9" s="37"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>278</v>
       </c>
@@ -3776,206 +3801,219 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>389</v>
+        <v>434</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>390</v>
-      </c>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>392</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
-        <v>280</v>
+        <v>391</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>393</v>
+        <v>280</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>394</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
-        <v>281</v>
+        <v>393</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="E22" s="25"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D23" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="E22" s="25"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="D23" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="37"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="37" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="37"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D25" s="5" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="D25" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="37"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C28" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D28" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="44"/>
+      <c r="E28" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3989,16 +4027,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="96.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4013,7 +4051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -4028,7 +4066,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4041,7 +4079,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>150</v>
       </c>
@@ -4058,7 +4096,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4071,7 +4109,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4084,7 +4122,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>127</v>
       </c>
@@ -4097,7 +4135,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4108,7 +4146,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4119,7 +4157,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4132,7 +4170,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4145,7 +4183,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -4158,7 +4196,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -4171,7 +4209,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -4184,7 +4222,7 @@
       </c>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>150</v>
       </c>
@@ -4201,7 +4239,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="33" t="s">
         <v>6</v>
@@ -4214,7 +4252,7 @@
       </c>
       <c r="E16" s="38"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="33" t="s">
         <v>12</v>
@@ -4227,7 +4265,7 @@
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>127</v>
       </c>
@@ -4240,7 +4278,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
@@ -4251,7 +4289,7 @@
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
@@ -4262,7 +4300,7 @@
       </c>
       <c r="E20" s="25"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="27"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
@@ -4275,7 +4313,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
@@ -4288,7 +4326,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
@@ -4301,7 +4339,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="34" t="s">
         <v>40</v>
@@ -4314,7 +4352,7 @@
       </c>
       <c r="E24" s="36"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="34" t="s">
         <v>7</v>
@@ -4327,7 +4365,7 @@
       </c>
       <c r="E25" s="36"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>127</v>
       </c>
@@ -4344,7 +4382,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="9" t="s">
         <v>6</v>
@@ -4357,7 +4395,7 @@
       </c>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>127</v>
       </c>
@@ -4370,7 +4408,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
@@ -4381,7 +4419,7 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
@@ -4392,7 +4430,7 @@
       </c>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="27"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
@@ -4405,7 +4443,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="24"/>
       <c r="C32" s="24" t="s">
@@ -4418,7 +4456,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>7</v>
@@ -4431,7 +4469,7 @@
       </c>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="43" t="s">
         <v>40</v>
@@ -4456,16 +4494,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4480,7 +4518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -4497,7 +4535,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4510,7 +4548,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>116</v>
       </c>
@@ -4527,7 +4565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -4540,7 +4578,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -4553,7 +4591,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>112</v>
       </c>
@@ -4566,7 +4604,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -4577,7 +4615,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -4588,7 +4626,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4599,7 +4637,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -4610,7 +4648,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
@@ -4625,7 +4663,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>5</v>
@@ -4640,7 +4678,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -4653,7 +4691,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -4666,7 +4704,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -4692,16 +4730,16 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -4716,7 +4754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
@@ -4731,7 +4769,7 @@
       </c>
       <c r="E2" s="43"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>12</v>
@@ -4744,7 +4782,7 @@
       </c>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>119</v>
       </c>
@@ -4761,7 +4799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -4774,7 +4812,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="11" t="s">
         <v>12</v>
@@ -4787,7 +4825,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>181</v>
       </c>
@@ -4800,7 +4838,7 @@
       </c>
       <c r="E7" s="30"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -4811,7 +4849,7 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -4822,7 +4860,7 @@
       </c>
       <c r="E9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -4833,7 +4871,7 @@
       </c>
       <c r="E10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -4844,7 +4882,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24" t="s">
@@ -4855,7 +4893,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
@@ -4866,7 +4904,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="24" t="s">
         <v>5</v>
@@ -4881,7 +4919,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="11" t="s">
         <v>40</v>
@@ -4894,7 +4932,7 @@
       </c>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="11" t="s">
         <v>7</v>
@@ -4905,7 +4943,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="49"/>
       <c r="B17" s="43" t="s">
         <v>40</v>
@@ -4930,16 +4968,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4954,7 +4992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -4969,7 +5007,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -4982,7 +5020,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>112</v>
       </c>
@@ -4999,7 +5037,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -5012,7 +5050,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -5025,7 +5063,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>97</v>
       </c>
@@ -5042,7 +5080,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5053,7 +5091,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5064,7 +5102,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5075,7 +5113,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5086,7 +5124,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -5097,7 +5135,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24" t="s">
@@ -5108,7 +5146,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23" t="s">
         <v>5</v>
@@ -5123,7 +5161,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>40</v>
@@ -5136,7 +5174,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>7</v>
@@ -5149,7 +5187,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="43" t="s">
         <v>40</v>
@@ -5173,16 +5211,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -5197,7 +5235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
@@ -5212,7 +5250,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5225,7 +5263,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>119</v>
       </c>
@@ -5242,7 +5280,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5255,7 +5293,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5268,7 +5306,7 @@
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>96</v>
       </c>
@@ -5285,7 +5323,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24" t="s">
@@ -5296,7 +5334,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
@@ -5307,7 +5345,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24" t="s">
@@ -5318,7 +5356,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24" t="s">
@@ -5329,7 +5367,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>5</v>
@@ -5344,7 +5382,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -5357,7 +5395,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>40</v>
@@ -5370,7 +5408,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -5383,7 +5421,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="43" t="s">
         <v>40</v>
@@ -5407,16 +5445,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5431,7 +5469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5448,7 +5486,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5461,7 +5499,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>221</v>
       </c>
@@ -5478,7 +5516,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5491,7 +5529,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5504,7 +5542,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>204</v>
       </c>
@@ -5517,7 +5555,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5528,7 +5566,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5539,7 +5577,7 @@
       </c>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5550,7 +5588,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5561,7 +5599,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -5572,7 +5610,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
@@ -5585,7 +5623,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>7</v>
@@ -5598,7 +5636,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
         <v>40</v>
@@ -5622,16 +5660,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5646,7 +5684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5663,7 +5701,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5676,7 +5714,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>222</v>
       </c>
@@ -5693,7 +5731,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5706,7 +5744,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5719,7 +5757,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>210</v>
       </c>
@@ -5732,7 +5770,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5743,7 +5781,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5756,7 +5794,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5769,7 +5807,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5780,7 +5818,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>40</v>
@@ -5793,7 +5831,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>7</v>
@@ -5806,7 +5844,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
         <v>40</v>
@@ -5831,16 +5869,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
-    <col min="4" max="4" width="78.5703125" customWidth="1"/>
-    <col min="5" max="5" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="4" width="78.5546875" customWidth="1"/>
+    <col min="5" max="5" width="92.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -5855,7 +5893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
@@ -5872,7 +5910,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="39" t="s">
         <v>12</v>
@@ -5885,7 +5923,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>323</v>
       </c>
@@ -5902,7 +5940,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -5915,7 +5953,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
         <v>12</v>
@@ -5928,7 +5966,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>344</v>
       </c>
@@ -5943,7 +5981,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -5954,7 +5992,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -5965,7 +6003,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -5976,7 +6014,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -5987,7 +6025,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -5998,7 +6036,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
@@ -6011,7 +6049,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
@@ -6022,7 +6060,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
@@ -6033,7 +6071,7 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>40</v>
@@ -6046,7 +6084,7 @@
       </c>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>7</v>
@@ -6059,7 +6097,7 @@
       </c>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
       <c r="B18" s="43" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
WADNR-2031 Add number part of Invoice "Organization Code" to report generator - Added OrganizationCodeValue and OrganizationCodeDisplay properties - Updated report model documentation
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
+++ b/Source/ProjectFirma.Web/Content/documents/Reports-Model-Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\WADNRForestHealth\Source\ProjectFirma.Web\Content\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E16EC34-6099-4783-BAC6-A3F5DDB553DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD087A8-3F75-46FD-B5F7-5E5A239156AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="5376" windowWidth="34560" windowHeight="18744" tabRatio="642" firstSheet="3" activeTab="11" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="642" xr2:uid="{F0F9A9E5-BBFB-400D-8D7D-8191321E58F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="442">
   <si>
     <t>Description of Field</t>
   </si>
@@ -1637,6 +1637,27 @@
   </si>
   <si>
     <t>InvoiceDateDisplay</t>
+  </si>
+  <si>
+    <t>OrganizationCodeValue</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.OrganizationCodeValue %&gt;</t>
+  </si>
+  <si>
+    <t>OrganizationCodeDisplay</t>
+  </si>
+  <si>
+    <t>&lt;%= invoice.OrganizationCodeDisplay %&gt;</t>
+  </si>
+  <si>
+    <t>e.g. 5900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.g. Forest Resilience Division </t>
+  </si>
+  <si>
+    <t>e.g. 5900 - Forest Resilience Division</t>
   </si>
 </sst>
 </file>
@@ -2234,7 +2255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD6FFD-16C8-4DD3-AED5-4AB2BB8A52D0}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3303,7 +3324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86115FEC-73BD-41B1-9C7A-4A7BD957B8AE}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3646,7 +3667,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F63DFE-4694-42F1-B8CF-3344A91DE8A8}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3899,43 +3920,49 @@
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24" t="s">
-        <v>284</v>
+        <v>435</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="E19" s="25"/>
+        <v>436</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="E20" s="25"/>
+        <v>294</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
-        <v>286</v>
+        <v>437</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="E21" s="25"/>
+        <v>438</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E22" s="25"/>
     </row>
@@ -3943,77 +3970,99 @@
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="E24" s="25"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D25" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37" t="s">
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C26" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D26" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="37"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37" t="s">
+      <c r="E26" s="37"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C27" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D27" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="37"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="E27" s="37"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
-      <c r="B28" s="43" t="s">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C30" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D30" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E30" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5658,7 +5707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62140-8660-4506-8649-E7BD6D8F000F}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>